<commit_message>
cleaning some more stuff up
</commit_message>
<xml_diff>
--- a/Projects/Project_5/game_four.xlsx
+++ b/Projects/Project_5/game_four.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22724"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="38" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A7361F24-0360-44FF-B109-586D705A6DC3}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16CAA5C2-02B1-425A-94CB-91729B30FDDC}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:F6"/>
+      <selection activeCell="F6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -476,26 +476,6 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>-10</v>
-      </c>
-      <c r="C6">
-        <v>-10</v>
-      </c>
-      <c r="D6">
-        <v>-10</v>
-      </c>
-      <c r="E6">
-        <v>-10</v>
-      </c>
-      <c r="F6">
-        <v>-10</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>